<commit_message>
Story 103: Added a test casses a document.
</commit_message>
<xml_diff>
--- a/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
+++ b/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Traceability_matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_cases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="158">
   <si>
     <t>Requirements document</t>
   </si>
@@ -320,13 +321,191 @@
   </si>
   <si>
     <t>6.5. Check that pages with standard errors have a friendly interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreConditions: </t>
+  </si>
+  <si>
+    <t>Test Case Description:</t>
+  </si>
+  <si>
+    <t>PostConditions:</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Test Result (passed/failed/blocked)</t>
+  </si>
+  <si>
+    <t>TC#1 Site header - Check the ability to select products and place an order.</t>
+  </si>
+  <si>
+    <t>1) An internet browser that supports an interface.
+2) The tested page is open in the browser, which is the only open tab.
+3) Russian is selected as the current language.</t>
+  </si>
+  <si>
+    <t>Selection of goods from the catalog and placing an order.</t>
+  </si>
+  <si>
+    <t>1) Cookies should be deleted after each test.
+2) Refresh the tab in the browser.
+3) If the user is on another page, he must return to the original.</t>
+  </si>
+  <si>
+    <t>Use a randomizer (preferably Random.org) to select the index number of the menu, page or product that will be used in the test (up to the maximum number of menu items, pages or products).</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Click on the menu item of the categories whose index you will get using step 1.</t>
+  </si>
+  <si>
+    <t>The page of the catalog of goods that apply only to the selected category has been posted.</t>
+  </si>
+  <si>
+    <t>Click on the menu item of the lower level categories, the serial number of which you will receive using step 1.</t>
+  </si>
+  <si>
+    <t>Click on the open submenu item whose index you will get using step 1.</t>
+  </si>
+  <si>
+    <t>The product catalog page has been posted, which applies only to the selected category and the corresponding page.</t>
+  </si>
+  <si>
+    <t>If a page list is displayed, click the page number whose number you will receive using step 1.</t>
+  </si>
+  <si>
+    <t>Click on the product name or image whose index you will get using step 1.</t>
+  </si>
+  <si>
+    <t>The product page has been loaded.</t>
+  </si>
+  <si>
+    <t>Click the Buy button.</t>
+  </si>
+  <si>
+    <t>In the Cart block in the header, the quantity and cost of the goods are added.</t>
+  </si>
+  <si>
+    <t>Repeat steps 2 to 7 at least 5 times to add another item to the cart.</t>
+  </si>
+  <si>
+    <t>In the “Cart” block in the header, the quantity and cost of the goods have changed accordingly.</t>
+  </si>
+  <si>
+    <t>Click the "Checkout" button in the header.</t>
+  </si>
+  <si>
+    <t>The cart page was loaded with the added products from step 7.</t>
+  </si>
+  <si>
+    <t>Increase the number of products in the last position by one and click the "Recalculate" button.</t>
+  </si>
+  <si>
+    <t>The quantity, value of goods and the total value in the basket have changed accordingly.</t>
+  </si>
+  <si>
+    <t>Click the “Place an order” button.</t>
+  </si>
+  <si>
+    <t>The order registration page has been loaded.</t>
+  </si>
+  <si>
+    <t>Try to enter data into all input fields from any test data set 1 and click “Submit”.</t>
+  </si>
+  <si>
+    <t>The order confirmation page has been posted.</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Open an email from Epicentrik at the email address specified in Test Dataset 1.</t>
+  </si>
+  <si>
+    <t>The letter should contain complete information about the order.</t>
+  </si>
+  <si>
+    <t>Open an email from Epicentrik that came to your Epicentrik email address.</t>
+  </si>
+  <si>
+    <t>Repeat Step from 1 to 14 with each of the 'correct' Test Data set 1</t>
+  </si>
+  <si>
+    <t>TC#3.3.2. - 3.3. Basket  -  Make sure that the correct data is transmitted in the field for entering the quantity of products.</t>
+  </si>
+  <si>
+    <t>Try changing the value in the field for entering the quantity of goods to a number from any test data set 2, marked as correct, and click the "Recalculate" button.</t>
+  </si>
+  <si>
+    <t>The field transmits data.</t>
+  </si>
+  <si>
+    <t>Repeat step 8 for each of the “correct” test data sets 2.</t>
+  </si>
+  <si>
+    <t>Try changing the value in the field for entering the quantity of goods to a number from any test data set 2, marked as incorrect, and click the "Recalculate" button.</t>
+  </si>
+  <si>
+    <t>No data is transferred to the field and a message is displayed asking for the correct data from the user.</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Repeat step 10 for each of the “wrong” test data sets 2.</t>
+  </si>
+  <si>
+    <t>TC#3.4.1. - 3.4. Checkout.  -   Make sure that order creation was successful only with complete and correct data.</t>
+  </si>
+  <si>
+    <t>Try to enter data into all input fields from any test data set 1, marked as correct, and click "Submit".</t>
+  </si>
+  <si>
+    <t>Repeat steps 1 through 8 for each “correct” test data set 1.</t>
+  </si>
+  <si>
+    <t>An order confirmation page has been posted</t>
+  </si>
+  <si>
+    <t>Try to enter data into all input fields from any set of test data marked as incorrect, and click "Submit".</t>
+  </si>
+  <si>
+    <t>A message is displayed with a description of the error.</t>
+  </si>
+  <si>
+    <t>Repeat steps 1 through 8 for each of the “wrong” test data sets 1.</t>
+  </si>
+  <si>
+    <t>TC#3.4.2. - 3.4. Checkout.  -   Check for error messages and their correctness when creating the order.</t>
+  </si>
+  <si>
+    <t>Try to enter data into all input fields from any test data set 1, marked as incorrect, and click "Submit".</t>
+  </si>
+  <si>
+    <t>TC#3.4.3. - 3.4. Checkout.  -   Check that the "Email" field is entered correctly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,8 +571,41 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,8 +618,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -596,47 +826,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -668,6 +1062,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,635 +1457,628 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
     </row>
     <row r="34" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
     </row>
     <row r="39" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
     </row>
     <row r="41" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A8:M8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="A38:M38"/>
     <mergeCell ref="B32:M32"/>
     <mergeCell ref="A21:M21"/>
     <mergeCell ref="B22:M22"/>
@@ -1599,15 +2091,22 @@
     <mergeCell ref="A29:M29"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="A31:M31"/>
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A12:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1618,8 +2117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B27"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,414 +2128,414 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="23"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="40" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="16" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="12" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="23" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
-      <c r="B32" s="23" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="4"/>
+      <c r="B34" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="4"/>
+      <c r="B35" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="22" t="s">
+      <c r="A36" s="4"/>
+      <c r="B36" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="17"/>
-      <c r="B37" s="23" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="22" t="s">
+      <c r="A39" s="4"/>
+      <c r="B39" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="22" t="s">
+      <c r="A40" s="4"/>
+      <c r="B40" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17"/>
-      <c r="B41" s="23" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="22" t="s">
+      <c r="A43" s="4"/>
+      <c r="B43" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="22" t="s">
+      <c r="A44" s="4"/>
+      <c r="B44" s="12" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="23" t="s">
+      <c r="A45" s="7"/>
+      <c r="B45" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="22" t="s">
+      <c r="A47" s="4"/>
+      <c r="B47" s="12" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="22" t="s">
+      <c r="A48" s="4"/>
+      <c r="B48" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="22" t="s">
+      <c r="A49" s="4"/>
+      <c r="B49" s="12" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17"/>
-      <c r="B50" s="23" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="22" t="s">
+      <c r="A52" s="4"/>
+      <c r="B52" s="12" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="22" t="s">
+      <c r="A53" s="4"/>
+      <c r="B53" s="12" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54" s="23" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="23" t="s">
+      <c r="A56" s="7"/>
+      <c r="B56" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="11" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="23" t="s">
+      <c r="A58" s="7"/>
+      <c r="B58" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="22" t="s">
+      <c r="A60" s="4"/>
+      <c r="B60" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="22" t="s">
+      <c r="A61" s="4"/>
+      <c r="B61" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="22" t="s">
+      <c r="A62" s="4"/>
+      <c r="B62" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="23" t="s">
+      <c r="A63" s="7"/>
+      <c r="B63" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2047,4 +2546,1157 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:E95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+    </row>
+    <row r="6" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+    </row>
+    <row r="7" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="44">
+        <v>2</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="44">
+        <v>3</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B12" s="46">
+        <v>4</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="46">
+        <v>5</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="46">
+        <v>6</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="46">
+        <v>7</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B16" s="46">
+        <v>8</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="46">
+        <v>9</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="46">
+        <v>10</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="46">
+        <v>11</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B20" s="46">
+        <v>12</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="46">
+        <v>13</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B22" s="46">
+        <v>14</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="46">
+        <v>15</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+    </row>
+    <row r="29" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+    </row>
+    <row r="30" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="44">
+        <v>1</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B33" s="44">
+        <v>2</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B34" s="44">
+        <v>3</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="46">
+        <v>4</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B36" s="46">
+        <v>5</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="46">
+        <v>6</v>
+      </c>
+      <c r="C37" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B38" s="46">
+        <v>7</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B39" s="46">
+        <v>8</v>
+      </c>
+      <c r="C39" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="46">
+        <v>9</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B41" s="46">
+        <v>10</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B42" s="46">
+        <v>11</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="29"/>
+    </row>
+    <row r="46" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="32"/>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="36"/>
+      <c r="E47" s="37"/>
+    </row>
+    <row r="48" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="36"/>
+      <c r="E48" s="37"/>
+    </row>
+    <row r="49" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="43"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B51" s="44">
+        <v>1</v>
+      </c>
+      <c r="C51" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B52" s="44">
+        <v>2</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B53" s="44">
+        <v>3</v>
+      </c>
+      <c r="C53" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B54" s="46">
+        <v>4</v>
+      </c>
+      <c r="C54" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E54" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B55" s="46">
+        <v>5</v>
+      </c>
+      <c r="C55" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E55" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="46">
+        <v>6</v>
+      </c>
+      <c r="C56" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B57" s="46">
+        <v>7</v>
+      </c>
+      <c r="C57" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D57" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B58" s="46">
+        <v>8</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="46">
+        <v>9</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E59" s="49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B60" s="46">
+        <v>10</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B61" s="46">
+        <v>11</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D61" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E61" s="49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="26"/>
+    </row>
+    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="27"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="29"/>
+    </row>
+    <row r="65" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="32"/>
+      <c r="E65" s="33"/>
+    </row>
+    <row r="66" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
+    </row>
+    <row r="67" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D67" s="36"/>
+      <c r="E67" s="37"/>
+    </row>
+    <row r="68" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="43"/>
+    </row>
+    <row r="69" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B70" s="44">
+        <v>1</v>
+      </c>
+      <c r="C70" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E70" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B71" s="44">
+        <v>2</v>
+      </c>
+      <c r="C71" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E71" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B72" s="44">
+        <v>3</v>
+      </c>
+      <c r="C72" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B73" s="46">
+        <v>4</v>
+      </c>
+      <c r="C73" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E73" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B74" s="46">
+        <v>5</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="46">
+        <v>6</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D75" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E75" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B76" s="46">
+        <v>7</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E76" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B77" s="46">
+        <v>8</v>
+      </c>
+      <c r="C77" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B78" s="46">
+        <v>9</v>
+      </c>
+      <c r="C78" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D78" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E78" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="26"/>
+    </row>
+    <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="29"/>
+    </row>
+    <row r="82" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D82" s="32"/>
+      <c r="E82" s="33"/>
+    </row>
+    <row r="83" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B83" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C83" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" s="36"/>
+      <c r="E83" s="37"/>
+    </row>
+    <row r="84" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D84" s="36"/>
+      <c r="E84" s="37"/>
+    </row>
+    <row r="85" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="43"/>
+    </row>
+    <row r="86" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D86" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="E86" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B87" s="44">
+        <v>1</v>
+      </c>
+      <c r="C87" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="E87" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B88" s="44">
+        <v>2</v>
+      </c>
+      <c r="C88" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="D88" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E88" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B89" s="44">
+        <v>3</v>
+      </c>
+      <c r="C89" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D89" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E89" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B90" s="46">
+        <v>4</v>
+      </c>
+      <c r="C90" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D90" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="E90" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B91" s="46">
+        <v>5</v>
+      </c>
+      <c r="C91" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E91" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B92" s="46">
+        <v>6</v>
+      </c>
+      <c r="C92" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E92" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B93" s="46">
+        <v>7</v>
+      </c>
+      <c r="C93" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D93" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="E93" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B94" s="46">
+        <v>8</v>
+      </c>
+      <c r="C94" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D94" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E94" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B95" s="46">
+        <v>9</v>
+      </c>
+      <c r="C95" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D95" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" s="49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B80:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B63:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B25:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B44:E45"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Story 104: Added a test data a document.
</commit_message>
<xml_diff>
--- a/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
+++ b/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Traceability_matrix" sheetId="2" r:id="rId2"/>
     <sheet name="Test_cases" sheetId="3" r:id="rId3"/>
+    <sheet name="Test_Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="197">
   <si>
     <t>Requirements document</t>
   </si>
@@ -499,13 +500,130 @@
   </si>
   <si>
     <t>TC#3.4.3. - 3.4. Checkout.  -   Check that the "Email" field is entered correctly.</t>
+  </si>
+  <si>
+    <t>Test Data Set 1: to create an order.</t>
+  </si>
+  <si>
+    <t>Test Data ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Сorrect</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>[void]</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;*()_+=,/&lt;&gt;?;\:"|[]{}`~0189</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>[default]</t>
+  </si>
+  <si>
+    <t>[наличный]</t>
+  </si>
+  <si>
+    <t>[безналичный]</t>
+  </si>
+  <si>
+    <t>[наложенный]</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>middle name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Payment method</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>Владислав</t>
+  </si>
+  <si>
+    <t>yellow@gmail.com</t>
+  </si>
+  <si>
+    <t>фіукпр .-'фіукпр .-'фіукпр .-'фіукпр .-'</t>
+  </si>
+  <si>
+    <t>yellow_qaQsd_dd@i.ua</t>
+  </si>
+  <si>
+    <t>фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189фіукпр .-'0189</t>
+  </si>
+  <si>
+    <t>Яблонская</t>
+  </si>
+  <si>
+    <t>Александра</t>
+  </si>
+  <si>
+    <t>Михайловна</t>
+  </si>
+  <si>
+    <t>yellow31031995_@gmail.com</t>
+  </si>
+  <si>
+    <t>+380508139348</t>
+  </si>
+  <si>
+    <t>Киев, ул. Анны Ахматовой 50, кв.63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">йцукерпавыфлчоосо 2 3 4 </t>
+  </si>
+  <si>
+    <t>Test Data Set 2: Type of product quantity.</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>-0.07</t>
+  </si>
+  <si>
+    <t>-1000000</t>
+  </si>
+  <si>
+    <t>Абвгд</t>
+  </si>
+  <si>
+    <t>Zxc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,6 +722,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1021,10 +1147,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1063,18 +1190,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1087,6 +1250,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1105,9 +1286,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1117,59 +1295,40 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1457,628 +1616,635 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
     </row>
     <row r="15" spans="1:13" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
     </row>
     <row r="20" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
     </row>
     <row r="22" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
     </row>
     <row r="24" spans="1:13" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
     </row>
     <row r="26" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:13" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
     </row>
     <row r="32" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
     </row>
     <row r="34" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
     </row>
     <row r="37" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
     </row>
     <row r="39" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
     </row>
     <row r="41" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A19:M19"/>
     <mergeCell ref="B32:M32"/>
     <mergeCell ref="A21:M21"/>
     <mergeCell ref="B22:M22"/>
@@ -2091,22 +2257,15 @@
     <mergeCell ref="A29:M29"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="A31:M31"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A8:M8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="A38:M38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2128,16 +2287,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="35"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2148,10 +2307,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2552,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B95" sqref="B95:E95"/>
     </sheetView>
   </sheetViews>
@@ -2566,1111 +2725,1128 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
     </row>
     <row r="4" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
     </row>
     <row r="6" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
     </row>
     <row r="7" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="44">
+      <c r="B9" s="21">
         <v>1</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="44">
+      <c r="B10" s="21">
         <v>2</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="44">
+      <c r="B11" s="21">
         <v>3</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="46">
+      <c r="B12" s="23">
         <v>4</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="46">
+      <c r="B13" s="23">
         <v>5</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="46">
+      <c r="B14" s="23">
         <v>6</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="46">
+      <c r="B15" s="23">
         <v>7</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B16" s="46">
+      <c r="B16" s="23">
         <v>8</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="49" t="s">
+      <c r="E16" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="46">
+      <c r="B17" s="23">
         <v>9</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="49" t="s">
+      <c r="E17" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B18" s="46">
+      <c r="B18" s="23">
         <v>10</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="49" t="s">
+      <c r="E18" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="46">
+      <c r="B19" s="23">
         <v>11</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="46">
+      <c r="B20" s="23">
         <v>12</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="46">
+      <c r="B21" s="23">
         <v>13</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="46">
+      <c r="B22" s="23">
         <v>14</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="46">
+      <c r="B23" s="23">
         <v>15</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="49" t="s">
+      <c r="E23" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="47"/>
     </row>
     <row r="27" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="33"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="50"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
     </row>
     <row r="30" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="44">
+      <c r="B32" s="21">
         <v>1</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="50" t="s">
+      <c r="D32" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B33" s="44">
+      <c r="B33" s="21">
         <v>2</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B34" s="44">
+      <c r="B34" s="21">
         <v>3</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B35" s="46">
+      <c r="B35" s="23">
         <v>4</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D35" s="47" t="s">
+      <c r="D35" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B36" s="46">
+      <c r="B36" s="23">
         <v>5</v>
       </c>
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D36" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="46">
+      <c r="B37" s="23">
         <v>6</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="D37" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B38" s="46">
+      <c r="B38" s="23">
         <v>7</v>
       </c>
-      <c r="C38" s="45" t="s">
+      <c r="C38" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="47" t="s">
+      <c r="D38" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="46">
+      <c r="B39" s="23">
         <v>8</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D39" s="47" t="s">
+      <c r="D39" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="46">
+      <c r="B40" s="23">
         <v>9</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C40" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B41" s="46">
+      <c r="B41" s="23">
         <v>10</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="45" t="s">
+      <c r="D41" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="26" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B42" s="46">
+      <c r="B42" s="23">
         <v>11</v>
       </c>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="26" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="26"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="44"/>
     </row>
     <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="47"/>
     </row>
     <row r="46" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="33"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="50"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="48" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="41"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="38" t="s">
+      <c r="E50" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="44">
+      <c r="B51" s="21">
         <v>1</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B52" s="44">
+      <c r="B52" s="21">
         <v>2</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="45" t="s">
+      <c r="D52" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="49" t="s">
+      <c r="E52" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B53" s="44">
+      <c r="B53" s="21">
         <v>3</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="45" t="s">
+      <c r="D53" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E53" s="49" t="s">
+      <c r="E53" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="54" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B54" s="46">
+      <c r="B54" s="23">
         <v>4</v>
       </c>
-      <c r="C54" s="45" t="s">
+      <c r="C54" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D54" s="45" t="s">
+      <c r="D54" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E54" s="49" t="s">
+      <c r="E54" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B55" s="46">
+      <c r="B55" s="23">
         <v>5</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="45" t="s">
+      <c r="D55" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="E55" s="49" t="s">
+      <c r="E55" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="46">
+      <c r="B56" s="23">
         <v>6</v>
       </c>
-      <c r="C56" s="45" t="s">
+      <c r="C56" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="45" t="s">
+      <c r="D56" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E56" s="49" t="s">
+      <c r="E56" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="46">
+      <c r="B57" s="23">
         <v>7</v>
       </c>
-      <c r="C57" s="45" t="s">
+      <c r="C57" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="45" t="s">
+      <c r="D57" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E57" s="49" t="s">
+      <c r="E57" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="58" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="46">
+      <c r="B58" s="23">
         <v>8</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C58" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D58" s="45" t="s">
+      <c r="D58" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="E58" s="49" t="s">
+      <c r="E58" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="59" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B59" s="46">
+      <c r="B59" s="23">
         <v>9</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C59" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="45" t="s">
+      <c r="D59" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="49" t="s">
+      <c r="E59" s="26" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="60" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B60" s="46">
+      <c r="B60" s="23">
         <v>10</v>
       </c>
-      <c r="C60" s="45" t="s">
+      <c r="C60" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="D60" s="45" t="s">
+      <c r="D60" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="26" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="61" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B61" s="46">
+      <c r="B61" s="23">
         <v>11</v>
       </c>
-      <c r="C61" s="45" t="s">
+      <c r="C61" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D61" s="45" t="s">
+      <c r="D61" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E61" s="49" t="s">
+      <c r="E61" s="26" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="26"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="44"/>
     </row>
     <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="27"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="29"/>
+      <c r="B64" s="45"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
+      <c r="E64" s="47"/>
     </row>
     <row r="65" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="C65" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="33"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="50"/>
     </row>
     <row r="66" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D66" s="36"/>
-      <c r="E66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="38"/>
     </row>
     <row r="67" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D67" s="36"/>
-      <c r="E67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="38"/>
     </row>
     <row r="68" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C68" s="42"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="43"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="41"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="38" t="s">
+      <c r="B69" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C69" s="38" t="s">
+      <c r="C69" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D69" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E69" s="38" t="s">
+      <c r="E69" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="44">
+      <c r="B70" s="21">
         <v>1</v>
       </c>
-      <c r="C70" s="45" t="s">
+      <c r="C70" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D70" s="50" t="s">
+      <c r="D70" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E70" s="49" t="s">
+      <c r="E70" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="71" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B71" s="44">
+      <c r="B71" s="21">
         <v>2</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D71" s="45" t="s">
+      <c r="D71" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E71" s="49" t="s">
+      <c r="E71" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B72" s="44">
+      <c r="B72" s="21">
         <v>3</v>
       </c>
-      <c r="C72" s="45" t="s">
+      <c r="C72" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D72" s="45" t="s">
+      <c r="D72" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E72" s="49" t="s">
+      <c r="E72" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B73" s="46">
+      <c r="B73" s="23">
         <v>4</v>
       </c>
-      <c r="C73" s="45" t="s">
+      <c r="C73" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D73" s="45" t="s">
+      <c r="D73" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E73" s="49" t="s">
+      <c r="E73" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="74" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B74" s="46">
+      <c r="B74" s="23">
         <v>5</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C74" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D74" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="E74" s="49" t="s">
+      <c r="E74" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="46">
+      <c r="B75" s="23">
         <v>6</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="C75" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D75" s="45" t="s">
+      <c r="D75" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E75" s="49" t="s">
+      <c r="E75" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="76" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B76" s="46">
+      <c r="B76" s="23">
         <v>7</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C76" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D76" s="45" t="s">
+      <c r="D76" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="49" t="s">
+      <c r="E76" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B77" s="46">
+      <c r="B77" s="23">
         <v>8</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C77" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="D77" s="45" t="s">
+      <c r="D77" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E77" s="49" t="s">
+      <c r="E77" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="78" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B78" s="46">
+      <c r="B78" s="23">
         <v>9</v>
       </c>
-      <c r="C78" s="45" t="s">
+      <c r="C78" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="45" t="s">
+      <c r="D78" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E78" s="49" t="s">
+      <c r="E78" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="24" t="s">
+      <c r="B80" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="26"/>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="44"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="27"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="29"/>
+      <c r="B81" s="45"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="47"/>
     </row>
     <row r="82" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C82" s="31" t="s">
+      <c r="C82" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="D82" s="32"/>
-      <c r="E82" s="33"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="50"/>
     </row>
     <row r="83" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="34" t="s">
+      <c r="B83" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D83" s="36"/>
-      <c r="E83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="38"/>
     </row>
     <row r="84" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="34" t="s">
+      <c r="B84" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C84" s="35" t="s">
+      <c r="C84" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D84" s="36"/>
-      <c r="E84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="38"/>
     </row>
     <row r="85" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="43"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
     </row>
     <row r="86" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B86" s="38" t="s">
+      <c r="B86" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="38" t="s">
+      <c r="C86" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D86" s="38" t="s">
+      <c r="D86" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E86" s="38" t="s">
+      <c r="E86" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="87" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B87" s="44">
+      <c r="B87" s="21">
         <v>1</v>
       </c>
-      <c r="C87" s="45" t="s">
+      <c r="C87" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D87" s="50" t="s">
+      <c r="D87" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E87" s="49" t="s">
+      <c r="E87" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="88" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B88" s="44">
+      <c r="B88" s="21">
         <v>2</v>
       </c>
-      <c r="C88" s="45" t="s">
+      <c r="C88" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="D88" s="45" t="s">
+      <c r="D88" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E88" s="49" t="s">
+      <c r="E88" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="89" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B89" s="44">
+      <c r="B89" s="21">
         <v>3</v>
       </c>
-      <c r="C89" s="45" t="s">
+      <c r="C89" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D89" s="45" t="s">
+      <c r="D89" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E89" s="49" t="s">
+      <c r="E89" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="90" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B90" s="46">
+      <c r="B90" s="23">
         <v>4</v>
       </c>
-      <c r="C90" s="45" t="s">
+      <c r="C90" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="D90" s="45" t="s">
+      <c r="D90" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E90" s="49" t="s">
+      <c r="E90" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="91" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B91" s="46">
+      <c r="B91" s="23">
         <v>5</v>
       </c>
-      <c r="C91" s="45" t="s">
+      <c r="C91" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="D91" s="45" t="s">
+      <c r="D91" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="E91" s="49" t="s">
+      <c r="E91" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="92" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B92" s="46">
+      <c r="B92" s="23">
         <v>6</v>
       </c>
-      <c r="C92" s="45" t="s">
+      <c r="C92" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D92" s="45" t="s">
+      <c r="D92" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="E92" s="49" t="s">
+      <c r="E92" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B93" s="46">
+      <c r="B93" s="23">
         <v>7</v>
       </c>
-      <c r="C93" s="45" t="s">
+      <c r="C93" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D93" s="45" t="s">
+      <c r="D93" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E93" s="49" t="s">
+      <c r="E93" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="94" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B94" s="46">
+      <c r="B94" s="23">
         <v>8</v>
       </c>
-      <c r="C94" s="45" t="s">
+      <c r="C94" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="D94" s="45" t="s">
+      <c r="D94" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E94" s="49" t="s">
+      <c r="E94" s="26" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="95" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B95" s="46">
+      <c r="B95" s="23">
         <v>9</v>
       </c>
-      <c r="C95" s="45" t="s">
+      <c r="C95" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D95" s="45" t="s">
+      <c r="D95" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E95" s="49" t="s">
+      <c r="E95" s="26" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B25:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B44:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B63:E64"/>
     <mergeCell ref="C84:E84"/>
     <mergeCell ref="B85:E85"/>
     <mergeCell ref="C66:E66"/>
@@ -3679,24 +3855,359 @@
     <mergeCell ref="B80:E81"/>
     <mergeCell ref="C82:E82"/>
     <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B63:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B25:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B44:E45"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="52">
+        <v>1</v>
+      </c>
+      <c r="C4" s="52">
+        <v>2</v>
+      </c>
+      <c r="D4" s="52">
+        <v>3</v>
+      </c>
+      <c r="E4" s="52">
+        <v>4</v>
+      </c>
+      <c r="F4" s="52">
+        <v>5</v>
+      </c>
+      <c r="G4" s="53">
+        <v>6</v>
+      </c>
+      <c r="H4" s="53">
+        <v>7</v>
+      </c>
+      <c r="J4" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" s="61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>163</v>
+      </c>
+      <c r="J5" s="53">
+        <v>1</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J6" s="53">
+        <v>10</v>
+      </c>
+      <c r="K6" s="55">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="53">
+        <v>99</v>
+      </c>
+      <c r="K7" s="55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J8" s="53">
+        <v>99999</v>
+      </c>
+      <c r="K8" s="55" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" s="53">
+        <v>1000000</v>
+      </c>
+      <c r="K9" s="55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="56">
+        <v>671234568</v>
+      </c>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" s="56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="C9" r:id="rId2"/>
+    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="F9" r:id="rId5"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Story 105: added a folder with screenshots.
</commit_message>
<xml_diff>
--- a/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
+++ b/Homework_6/Epicentr_Vlad_Dmytrenko.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Traceability_matrix" sheetId="2" r:id="rId2"/>
     <sheet name="Test_cases" sheetId="3" r:id="rId3"/>
     <sheet name="Test_Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Bug_report" sheetId="5" r:id="rId5"/>
+    <sheet name="Date" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="381">
   <si>
     <t>Requirements document</t>
   </si>
@@ -617,13 +619,565 @@
   </si>
   <si>
     <t>Zxc</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Reproducibility</t>
+  </si>
+  <si>
+    <t>Reporter</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected results</t>
+  </si>
+  <si>
+    <t>Steps to reproduce</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Created at</t>
+  </si>
+  <si>
+    <t>Updated at</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>v1.0</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Sometimes</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Acknowledged</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Visual</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>User input data</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Suggestion</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>There is no way to sort the goods in the catalog.</t>
+  </si>
+  <si>
+    <t>vladyslav</t>
+  </si>
+  <si>
+    <t>Sorting in the catalog should be by popularity, price, alphabet, novelty.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (if necessary); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header.</t>
+  </si>
+  <si>
+    <t>Windows PC Asus Generic/All Windows 7 Chrome Latest</t>
+  </si>
+  <si>
+    <t>HTTPS is not used</t>
+  </si>
+  <si>
+    <t>The site must use the https protocol</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open epicentrik.info</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:21</t>
+  </si>
+  <si>
+    <t>Incorrect display of the value of the search field in the header</t>
+  </si>
+  <si>
+    <t>The value of the search field in the header must be aligned according to requirement 1.4.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:24</t>
+  </si>
+  <si>
+    <t>An empty search message sent using the Enter key loads the Home page.</t>
+  </si>
+  <si>
+    <t>The last page should remain.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Go to any page except the "Home" page; 4. Place the mouse cursor in the search field and press the Enter key.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:29</t>
+  </si>
+  <si>
+    <t>Incorrect display of goods in the "Recommended Products" carousel on the main page.</t>
+  </si>
+  <si>
+    <t>Items in the Featured Products carousel on the Home page must be aligned with each other.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:32</t>
+  </si>
+  <si>
+    <t>Incorrect display of the site language switch in the header.</t>
+  </si>
+  <si>
+    <t>The link "RU" should be displayed in capital letters and lowercase letters "ua" when loading a page in Russian. When loading a page in Ukrainian, the link “ru” should be displayed in lowercase letters and capital letters “UA”.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on the “ua” link in the header.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:34</t>
+  </si>
+  <si>
+    <t>There is no translation of the names of the elements in the “Basket” block in the header in Ukrainian.</t>
+  </si>
+  <si>
+    <t>The names of the elements should be as follows: the names of the text fields “Your cat” and “Products for the bag”, the button “Place an order”.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:35</t>
+  </si>
+  <si>
+    <t>The lack of mandatory categories in the header in Ukrainian.</t>
+  </si>
+  <si>
+    <t>The categories menu contains the following categories: “Materials”, “Ozdoblyuvnye materials”, “Tools”, “Pidlog”, “Electrical goods”, “Plumbing”, “Pobutova technique”, “Garden and city”.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:37</t>
+  </si>
+  <si>
+    <t>There is no translation of the names of the carousels on the “Main” page in Ukrainian.</t>
+  </si>
+  <si>
+    <t>The names of the roundabouts on the “Main” page in Ukrainian should be: “Novi nadhodzhennya”, “People’s comrades”.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:39</t>
+  </si>
+  <si>
+    <t>There is no translation of the product name and description into Ukrainian in the product catalog and on the product page.</t>
+  </si>
+  <si>
+    <t>All product names and descriptions should be translated into Ukrainian.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click the "ua" link in the header; 4. Click on any product category; 5. Click on any product.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:41</t>
+  </si>
+  <si>
+    <t>There is no translation of the Buy button of a product into Ukrainian in the product catalog and on the product page.</t>
+  </si>
+  <si>
+    <t>The name of the button should be “Buy.”</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:43</t>
+  </si>
+  <si>
+    <t>Grammatical error in the link “Site map” in the footer.</t>
+  </si>
+  <si>
+    <t>The name of the link should be “Site Map”.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:44</t>
+  </si>
+  <si>
+    <t>Incorrect translation of the site map page name into Ukrainian.</t>
+  </si>
+  <si>
+    <t>The name of the page should be “Site Map”.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click the "ua" link in the header; 4. Click the “Site Map” icon in the header.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:46</t>
+  </si>
+  <si>
+    <t>There is no translation of the name of the page "Koshik" and its elements into Ukrainian.</t>
+  </si>
+  <si>
+    <t>The names of the page elements should be in Ukrainian, with or without added goods.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click the "ua" link in the header; 4. Click on any product category; 5. Click the Buy button on any product.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:48</t>
+  </si>
+  <si>
+    <t>There is no translation of the name of the page "Place an order" and its elements into Ukrainian.</t>
+  </si>
+  <si>
+    <t>The names of the page elements must be in Ukrainian.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click the "ua" link in the header; 4. Click on any item in the category menu at any level; 5. Press the "Buy" button on any product; 6. Click on the “Place an order” button.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:54</t>
+  </si>
+  <si>
+    <t>Wrong button "Home" in the site menu in the header.</t>
+  </si>
+  <si>
+    <t>URL epicentrik.info/en/city/266.html</t>
+  </si>
+  <si>
+    <t>Press the "Home" button, the header should contain the epicentrik.info download page.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click the "Home" button in the site menu in the / header</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:56</t>
+  </si>
+  <si>
+    <t>Wrong "Main" button in the site menu in the footer.</t>
+  </si>
+  <si>
+    <t>URL epicentrik.info/en/pages/2.htm</t>
+  </si>
+  <si>
+    <t>Click the Home button in the footer of the epicentrik.info download page.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on the “Home” button in the site menu in the footer.</t>
+  </si>
+  <si>
+    <t>11.10.2019.22:58</t>
+  </si>
+  <si>
+    <t>Incorrect display of the order of items in the lower level category menu.</t>
+  </si>
+  <si>
+    <t>Category menu items should be displayed in alphabetical order.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Click on any item in the lower level category menu.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:00</t>
+  </si>
+  <si>
+    <t>Incorrect display of goods in the catalog.</t>
+  </si>
+  <si>
+    <t>Items in the catalog must be aligned with each other.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:02</t>
+  </si>
+  <si>
+    <t>Incorrect display of navigation on catalog pages.</t>
+  </si>
+  <si>
+    <t>Navigation in the catalog pages should display the number of the current page and links to the first, neighboring, last pages.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:04</t>
+  </si>
+  <si>
+    <t>Incorrect processing of data entered in the "Quantity" field on the "Basket" page.</t>
+  </si>
+  <si>
+    <t>The Quantity field should only accept positive integers.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Press the "Buy" button on any product; 5. Click the "Place an order" button in the header; 6. Enter a negative value in the “Quantity” text box and click the “Recalculate” button; 7. Repeat steps 3 to 5 to add another item to the cart; 8. Enter the fractional value in the “Quantity” text box opposite the last added product and click the “Recalculate” button.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:06</t>
+  </si>
+  <si>
+    <t>Incorrect processing of data entered in the "Name" field on the "Basket" page.</t>
+  </si>
+  <si>
+    <t>Order does not have to be completed. If you enter incorrect data in the "Name" field, an error should be displayed.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Press the Buy button on any product; 5. Click the "Place an order" button in the header; 6. Click the "Place an order" button in the content area; 7. Enter the value "! @ # $% ^ &amp; * () _ + =, / &lt;&gt;?; \:" | [] {} `~ 0189" in the "Name" field; 8. Click the "Submit" button in the content area.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:08</t>
+  </si>
+  <si>
+    <t>There are no values in the "Payment method:" drop-down list on the "Place an order" page.</t>
+  </si>
+  <si>
+    <t>The drop-down list “Payment method:” should contain the following items: “choose a method” (default), “cash”, “non-cash”, “cash on delivery”.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Press the Buy button on any product; 5. Click the "Place an order" button in the header; 6. Click on the “Checkout” button in the content area.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:10</t>
+  </si>
+  <si>
+    <t>The absence of signs of required fields for filling out the feedback form on the Contact page.</t>
+  </si>
+  <si>
+    <t>Mandatory fields must be marked with an asterisk.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click "Contacts" in the site menu.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:11</t>
+  </si>
+  <si>
+    <t>Incorrect processing of data entered in the "Name" field on the "Contacts" page.</t>
+  </si>
+  <si>
+    <t>Sending must not be completed. An error should be displayed about entering incorrect data in the "Имя" field.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click "Contacts" in the site menu; 4. Enter the value '! @ # $% ^ &amp; * () _ + =, / &lt;&gt;?; \: "| [] {}` ~ 0189 'in the field "Name"; 5. Enter the value "igor@i.ua" in the field "Your e-mail:"; 6. Enter the value "question" in "Question: "; 7. Enter the correct solution of the equation in the captcha field; 8. Click the" Submit "button in the content area.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:15</t>
+  </si>
+  <si>
+    <t>Lack of emphasis on the Buy buttons on the catalog page and product page.</t>
+  </si>
+  <si>
+    <t>Focus on the Buy buttons using the Tab and Shift + Tab buttons on the product catalog page and product page.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Press the “Tab” or “Shift + Tab” buttons until the “Buy” button is focused; 5. Click on any product and repeat step 4.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:16</t>
+  </si>
+  <si>
+    <t>Incorrect focus on a non-displayable item.</t>
+  </si>
+  <si>
+    <t>Focus should only be on the displayed items.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Press the "Tab" or "Shift + Tab" buttons until the focus moves to the element with the link epicentrik.info/#js-p2018-sidebar.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:18</t>
+  </si>
+  <si>
+    <t>Download the link and the JS script with errors.</t>
+  </si>
+  <si>
+    <t>The code should not contain broken links and invalid JS scripts.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. View code errors using the developer tools or manually.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:20</t>
+  </si>
+  <si>
+    <t>There is no indentation between the "Recalculate", "Clear", "Checkout" buttons and the footer.</t>
+  </si>
+  <si>
+    <t>There is no indentation between the buttons "Recalculate", "Clear", "Place an order" and the footer on the page "Basket" with more than 4 products.</t>
+  </si>
+  <si>
+    <t>The margins from the header and footer to the content area are visually identical.</t>
+  </si>
+  <si>
+    <t>1. Launch an Internet browser that supports the interface (as required); 2. In the browser, open the epicentrik.info page; 3. Click on any item in the category menu in the header; 4. Press the Buy button on any product; 5. Repeat steps 3 to 5 at least 5 times to add another product to the basket; 6. Click the "Place an order" button in the header.</t>
+  </si>
+  <si>
+    <t>11.10.2019.23:21</t>
+  </si>
+  <si>
+    <t>The HTTPS protocol is not used according to requirement 5. The error visualization is located in the attached file "page_1.jpg".</t>
+  </si>
+  <si>
+    <t>The value of the search field in the header is not aligned according to requirement 1.4. The error is marked with a red circle in the attached file "page_2.jpg"</t>
+  </si>
+  <si>
+    <t>Items in the Featured Products carousel on the Home page are not aligned with each other. Error visualization is in the attached file "page_3.jpg".</t>
+  </si>
+  <si>
+    <t>Links "RU" and "UA" are displayed in capital letters when loading a page in Russian. Links "RU" and "UA" are displayed in lowercase letters when loading a page in Ukrainian. Error visualization is located in the attached files "page_4.1.jpg" and "page_4.2.jpg".</t>
+  </si>
+  <si>
+    <t>The names of the elements are as follows: the names of the text fields “Your basket” and “Total goods”, the button “Place an order”. Error visualization is in the attached file "page_5.jpg"</t>
+  </si>
+  <si>
+    <t>The following categories are not present in the categories menu: “Pobutova Technology”, “Garden and City”. Error visualization is located in the attached file "page_6.jpg".</t>
+  </si>
+  <si>
+    <t>The names of the carousels on the "Main" page in Ukrainian are as follows: "New arrivals", "Popular comrades." The error visualization is in the attached file "page_7.jpg".</t>
+  </si>
+  <si>
+    <t>All product names and descriptions are not translated into Ukrainian. Error visualization is located in the attached files "page_8.jpg".</t>
+  </si>
+  <si>
+    <t>The name of the Buy button. The error visualization is located in the attached file "page_9.jpg".</t>
+  </si>
+  <si>
+    <t>The name of the link is “Site Map”. The error is marked with a red circle in the attached file "Page_10.jpg.</t>
+  </si>
+  <si>
+    <t>The name of the page is “SITE MAP”. The error is marked with a red circle in the attached file "page_11.1.jpg" and "page_11.2.jpg".</t>
+  </si>
+  <si>
+    <t>The names of the page elements are not in Ukrainian, both with or without added goods. Error visualization is located in the attached files "page_12.1.jpg" and "page_12.2.jpg".</t>
+  </si>
+  <si>
+    <t>The names of the page elements are not in Ukrainian. The error is marked with a red circle in the attached file "page_12.1.jpg".</t>
+  </si>
+  <si>
+    <t>Category menu items are not displayed in alphabetical order. The error is marked with a red circle in the attached file "page_13.jpg".</t>
+  </si>
+  <si>
+    <t>Items in the catalog are not aligned with each other. Error visualization is in the attached file "page_14.jpg".</t>
+  </si>
+  <si>
+    <t>Navigating through catalog pages is not convenient to use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no sorting option in the catalog. </t>
+  </si>
+  <si>
+    <t>The Number field accepts negative and fractional numbers. The error visualization is located in the attached file "page_15.jpg".</t>
+  </si>
+  <si>
+    <t>Your order has been completed. The Number field accepts brackets, special characters, etc., In addition to dashes, letters, spaces, periods. The error visualization is located in the attached file "page_16.jpg".</t>
+  </si>
+  <si>
+    <t>The drop-down list “Payment method:” does not contain mandatory items. Error visualization is in the attached file "page_17.jpg".</t>
+  </si>
+  <si>
+    <t>Required fields are not marked with an asterisk. The error visualization is located in the attached file "page_18.jpg".</t>
+  </si>
+  <si>
+    <t>Your message has been sent. The “Name” field takes brackets, special characters, etc., In addition to dashes, letters, spaces, periods. Error visualization is in the attached file "page_19.1.jpg" and "page_19.2.jpg".</t>
+  </si>
+  <si>
+    <t>Lack of focus on the Buy buttons using the Tab and Shift + Tab buttons on the product catalog page and product page.</t>
+  </si>
+  <si>
+    <t>The focus is on the non-displayable item between the Contact button in the header and the navigation tree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The code contains broken links and invalid JS scripts. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,8 +1284,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,8 +1330,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1146,12 +1720,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1226,78 +1883,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1326,10 +1911,125 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1609,642 +2309,635 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="55"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
     </row>
     <row r="15" spans="1:13" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
     </row>
     <row r="20" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
     </row>
     <row r="22" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
     </row>
     <row r="24" spans="1:13" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
     </row>
     <row r="26" spans="1:13" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
     </row>
     <row r="28" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
     </row>
     <row r="30" spans="1:13" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="55"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
     </row>
     <row r="32" spans="1:13" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="55"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="55"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
     </row>
     <row r="34" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="54"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
     </row>
     <row r="37" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="55"/>
+      <c r="M37" s="55"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-      <c r="L38" s="29"/>
-      <c r="M38" s="29"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
     </row>
     <row r="39" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="54"/>
     </row>
     <row r="41" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="55"/>
+      <c r="M41" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A8:M8"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="A38:M38"/>
     <mergeCell ref="B32:M32"/>
     <mergeCell ref="A21:M21"/>
     <mergeCell ref="B22:M22"/>
@@ -2257,15 +2950,22 @@
     <mergeCell ref="A29:M29"/>
     <mergeCell ref="B30:M30"/>
     <mergeCell ref="A31:M31"/>
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A12:M12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2276,7 +2976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -2287,16 +2987,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
+      <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -2711,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B95" sqref="B95:E95"/>
     </sheetView>
   </sheetViews>
@@ -2725,56 +3425,56 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65"/>
     </row>
     <row r="4" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="50"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="6" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="71"/>
     </row>
     <row r="7" spans="2:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="74"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
@@ -3002,56 +3702,56 @@
     </row>
     <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
     </row>
     <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="45"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
     </row>
     <row r="27" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="50"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
     </row>
     <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
     </row>
     <row r="29" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
     </row>
     <row r="30" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="41"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="74"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
@@ -3223,56 +3923,56 @@
     </row>
     <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="44"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
     </row>
     <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="45"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="47"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="65"/>
     </row>
     <row r="46" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="50"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="68"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="36" t="s">
+      <c r="C47" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="37"/>
-      <c r="E47" s="38"/>
+      <c r="D47" s="70"/>
+      <c r="E47" s="71"/>
     </row>
     <row r="48" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="71"/>
     </row>
     <row r="49" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="41"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="74"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
@@ -3444,56 +4144,56 @@
     </row>
     <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="42" t="s">
+      <c r="B63" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="C63" s="43"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="44"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="62"/>
     </row>
     <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="45"/>
-      <c r="C64" s="46"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="47"/>
+      <c r="B64" s="63"/>
+      <c r="C64" s="64"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="65"/>
     </row>
     <row r="65" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="48" t="s">
+      <c r="C65" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D65" s="49"/>
-      <c r="E65" s="50"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="68"/>
     </row>
     <row r="66" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D66" s="37"/>
-      <c r="E66" s="38"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="71"/>
     </row>
     <row r="67" spans="2:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D67" s="37"/>
-      <c r="E67" s="38"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="71"/>
     </row>
     <row r="68" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="39" t="s">
+      <c r="B68" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="41"/>
+      <c r="C68" s="73"/>
+      <c r="D68" s="73"/>
+      <c r="E68" s="74"/>
     </row>
     <row r="69" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="18" t="s">
@@ -3637,56 +4337,56 @@
     </row>
     <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="42" t="s">
+      <c r="B80" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="44"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="62"/>
     </row>
     <row r="81" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="45"/>
-      <c r="C81" s="46"/>
-      <c r="D81" s="46"/>
-      <c r="E81" s="47"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="65"/>
     </row>
     <row r="82" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C82" s="48" t="s">
+      <c r="C82" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="D82" s="49"/>
-      <c r="E82" s="50"/>
+      <c r="D82" s="67"/>
+      <c r="E82" s="68"/>
     </row>
     <row r="83" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C83" s="36" t="s">
+      <c r="C83" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D83" s="37"/>
-      <c r="E83" s="38"/>
+      <c r="D83" s="70"/>
+      <c r="E83" s="71"/>
     </row>
     <row r="84" spans="2:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C84" s="36" t="s">
+      <c r="C84" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="D84" s="37"/>
-      <c r="E84" s="38"/>
+      <c r="D84" s="70"/>
+      <c r="E84" s="71"/>
     </row>
     <row r="85" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B85" s="39" t="s">
+      <c r="B85" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
+      <c r="C85" s="73"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="74"/>
     </row>
     <row r="86" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
@@ -3830,11 +4530,14 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B80:E81"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="C83:E83"/>
     <mergeCell ref="C65:E65"/>
     <mergeCell ref="B25:E26"/>
     <mergeCell ref="C27:E27"/>
@@ -3847,14 +4550,11 @@
     <mergeCell ref="C48:E48"/>
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="B63:E64"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B80:E81"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3864,7 +4564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -3883,315 +4583,315 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="75" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="36" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="28">
         <v>1</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="28">
         <v>2</v>
       </c>
-      <c r="D4" s="52">
+      <c r="D4" s="28">
         <v>3</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="28">
         <v>4</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="28">
         <v>5</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="29">
         <v>6</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="29">
         <v>7</v>
       </c>
-      <c r="J4" s="61" t="s">
+      <c r="J4" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="K4" s="61" t="s">
+      <c r="K4" s="37" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="29">
         <v>1</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="31" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="J6" s="53">
+      <c r="J6" s="29">
         <v>10</v>
       </c>
-      <c r="K6" s="55">
+      <c r="K6" s="31">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="J7" s="53">
+      <c r="J7" s="29">
         <v>99</v>
       </c>
-      <c r="K7" s="55" t="s">
+      <c r="K7" s="31" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="56" t="s">
+      <c r="H8" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="J8" s="53">
+      <c r="J8" s="29">
         <v>99999</v>
       </c>
-      <c r="K8" s="55" t="s">
+      <c r="K8" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="H9" s="56" t="s">
+      <c r="H9" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="J9" s="53">
+      <c r="J9" s="29">
         <v>1000000</v>
       </c>
-      <c r="K9" s="55" t="s">
+      <c r="K9" s="31" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="32">
         <v>671234568</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53" t="s">
+      <c r="J10" s="29"/>
+      <c r="K10" s="29" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="G11" s="56" t="s">
+      <c r="G11" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="55" t="s">
+      <c r="J11" s="30"/>
+      <c r="K11" s="31" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="H12" s="32" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="56" t="s">
+      <c r="G13" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="56" t="s">
+      <c r="H13" s="32" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4210,4 +4910,1688 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="36" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" customWidth="1"/>
+    <col min="13" max="13" width="35.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="O1" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="P1" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q1" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="R1" s="38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="R2" s="30"/>
+    </row>
+    <row r="3" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J3" s="30"/>
+      <c r="K3" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="R3" s="30"/>
+    </row>
+    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="R5" s="30"/>
+    </row>
+    <row r="6" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="R6" s="30"/>
+    </row>
+    <row r="7" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="22" t="s">
+        <v>360</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="R7" s="30"/>
+    </row>
+    <row r="8" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="R9" s="30"/>
+    </row>
+    <row r="10" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="R10" s="30"/>
+    </row>
+    <row r="11" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="R11" s="30"/>
+    </row>
+    <row r="12" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J12" s="25"/>
+      <c r="K12" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="R12" s="30"/>
+    </row>
+    <row r="13" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="R13" s="30"/>
+    </row>
+    <row r="14" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="R14" s="30"/>
+    </row>
+    <row r="15" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="22" t="s">
+        <v>368</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="R15" s="30"/>
+    </row>
+    <row r="16" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J16" s="25"/>
+      <c r="K16" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="R16" s="30"/>
+    </row>
+    <row r="17" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>306</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="R17" s="30"/>
+    </row>
+    <row r="18" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="22" t="s">
+        <v>369</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="R18" s="30"/>
+    </row>
+    <row r="19" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="R19" s="30"/>
+    </row>
+    <row r="20" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
+        <v>19</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="22" t="s">
+        <v>371</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="R20" s="30"/>
+    </row>
+    <row r="21" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="M21" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="51">
+        <v>43748.518055555556</v>
+      </c>
+      <c r="R21" s="30"/>
+    </row>
+    <row r="22" spans="1:18" ht="225" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="22" t="s">
+        <v>373</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="M22" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="R22" s="30"/>
+    </row>
+    <row r="23" spans="1:18" ht="195" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <v>22</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="R23" s="30"/>
+    </row>
+    <row r="24" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <v>23</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="R24" s="30"/>
+    </row>
+    <row r="25" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J25" s="25"/>
+      <c r="K25" s="22" t="s">
+        <v>376</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="R25" s="30"/>
+    </row>
+    <row r="26" spans="1:18" ht="195" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>25</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J26" s="25"/>
+      <c r="K26" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="M26" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="R26" s="30"/>
+    </row>
+    <row r="27" spans="1:18" ht="135" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>26</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J27" s="25"/>
+      <c r="K27" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="N27" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="R27" s="30"/>
+    </row>
+    <row r="28" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>27</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J28" s="25"/>
+      <c r="K28" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="L28" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="N28" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="R28" s="30"/>
+    </row>
+    <row r="29" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="25">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J29" s="25"/>
+      <c r="K29" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="L29" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="M29" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="N29" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O29" s="25"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="R29" s="25"/>
+    </row>
+    <row r="30" spans="1:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>29</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J30" s="25"/>
+      <c r="K30" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="M30" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="N30" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="R30" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$B$2:$B$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$C$2:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$D$2:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$E$2:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G30</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Date!$F$2:$F$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H30</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
+      <c r="B3" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="48"/>
+      <c r="B5" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" s="48"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="48"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="F7" s="49"/>
+      <c r="G7" s="48"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>